<commit_message>
mailList and data formatted
</commit_message>
<xml_diff>
--- a/config/sample.xlsx
+++ b/config/sample.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KH160\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\planning-sheet\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0964A68C-7D7E-4B97-9A2E-3EE9A301A35E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{481E9FFC-3EC1-4CBA-9417-4314B2B0400E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{2B7FBB39-1141-4963-9ABE-2FC05CD16186}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{2B7FBB39-1141-4963-9ABE-2FC05CD16186}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="milestones" sheetId="1" r:id="rId1"/>
+    <sheet name="mails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="107">
   <si>
     <t>Milestones</t>
   </si>
@@ -135,9 +136,6 @@
     <t>25th Oct</t>
   </si>
   <si>
-    <t>19th / 22nd Oct</t>
-  </si>
-  <si>
     <t>60 % PRD readiness for M4</t>
   </si>
   <si>
@@ -316,13 +314,46 @@
   </si>
   <si>
     <t>Code completion</t>
+  </si>
+  <si>
+    <t>22nd Oct</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t>PRD</t>
+  </si>
+  <si>
+    <t>pm@kony.com</t>
+  </si>
+  <si>
+    <t>ux@kony.com</t>
+  </si>
+  <si>
+    <t>doc@kony.com</t>
+  </si>
+  <si>
+    <t>prd@kony.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +388,14 @@
       <color rgb="FFC65911"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -487,10 +526,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -521,6 +561,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,11 +586,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -864,8 +907,8 @@
   </sheetPr>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +946,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +957,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,7 +989,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
@@ -987,7 +1030,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>27</v>
@@ -1002,7 +1045,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1019,7 +1062,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -1052,7 +1095,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>30</v>
@@ -1087,99 +1130,99 @@
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="6"/>
     </row>
@@ -1190,183 +1233,183 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="17"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="C46" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>96</v>
+      <c r="A55" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" s="6"/>
     </row>
@@ -1375,23 +1418,23 @@
         <v>3</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
+      <c r="A57" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="19"/>
+      <c r="C57" s="20"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="C58" s="6"/>
     </row>
@@ -1400,7 +1443,7 @@
         <v>4</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="6"/>
     </row>
@@ -1413,4 +1456,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83DB8BE-9AAD-42F4-99D1-485271FE9F83}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{60E92FB8-1735-4AEC-A508-C49B9888EB37}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8028E354-237C-4175-8BE4-D43EDD687510}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{799DBD05-EDFA-4A2F-B55A-568E65D5F9CD}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{D07493D2-157B-4A01-A6C7-0414FAD15947}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>